<commit_message>
Changes to CPIC Wizard
</commit_message>
<xml_diff>
--- a/UGT1A1_Diplotype_Phenotype_Table.xlsx
+++ b/UGT1A1_Diplotype_Phenotype_Table.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koki/KGrid_files/CPIC_Gene_Diplotype_Phenotype_Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koki/KGrid_files/CPIC-objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16940" yWindow="460" windowWidth="16800" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="5000" yWindow="7080" windowWidth="33600" windowHeight="19580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Possible UGT1A1 Diplotype" sheetId="6" r:id="rId1"/>
@@ -239,6 +239,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>a</t>
@@ -284,6 +285,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">UGT1A1 </t>
@@ -304,6 +306,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">UGT1A1 </t>
@@ -380,6 +383,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>c</t>
@@ -394,6 +398,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Term changed from guideline based on CPIC Term Standardization Project</t>
@@ -408,6 +413,7 @@
         <sz val="12"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>Term changed from guideline based on CPIC Term Standardization Project</t>
@@ -423,6 +429,7 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </rPr>
       <t>d</t>
@@ -486,12 +493,14 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -499,6 +508,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -507,6 +517,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -514,6 +525,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -521,6 +533,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1525,9 +1538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1547,7 +1558,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1558,7 +1569,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1569,7 +1580,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -1580,7 +1591,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
@@ -1591,7 +1602,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
@@ -1602,7 +1613,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>1</v>
       </c>
@@ -1613,7 +1624,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>21</v>
       </c>
@@ -1624,7 +1635,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
@@ -1635,7 +1646,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1646,7 +1657,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1657,7 +1668,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1668,7 +1679,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
@@ -1679,7 +1690,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -1690,7 +1701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
@@ -1701,7 +1712,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
@@ -1712,7 +1723,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>23</v>
       </c>
@@ -1723,7 +1734,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>18</v>
       </c>
@@ -1734,7 +1745,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
@@ -1745,7 +1756,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
         <v>24</v>
       </c>
@@ -1756,7 +1767,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>20</v>
       </c>
@@ -1767,7 +1778,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
         <v>25</v>
       </c>
@@ -1778,7 +1789,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>7</v>
       </c>
@@ -1789,7 +1800,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>8</v>
       </c>
@@ -1800,7 +1811,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>9</v>
       </c>
@@ -1811,7 +1822,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>10</v>
       </c>
@@ -1822,7 +1833,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>6</v>
       </c>
@@ -1833,7 +1844,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
@@ -1844,7 +1855,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>

</xml_diff>